<commit_message>
Corrected wrong time vector in data file
</commit_message>
<xml_diff>
--- a/data/2017-08-18_seq8_Huh7_eGFP_CHX.xlsx
+++ b/data/2017-08-18_seq8_Huh7_eGFP_CHX.xlsx
@@ -134,7 +134,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -918,9 +918,9 @@
         <v>-0.047</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-0.038</v>
@@ -1310,9 +1310,9 @@
         <v>0.003</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-0.005</v>
@@ -1702,9 +1702,9 @@
         <v>0.163</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.002</v>
@@ -2094,9 +2094,9 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-0.145</v>
@@ -2486,9 +2486,9 @@
         <v>0.013</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-0.235</v>
@@ -2878,9 +2878,9 @@
         <v>-0.038</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-0.233</v>
@@ -3270,9 +3270,9 @@
         <v>0.044</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>1.4</v>
+        <v>1.75</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.019</v>
@@ -3662,9 +3662,9 @@
         <v>0.076</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-0.082</v>
@@ -4054,9 +4054,9 @@
         <v>-0.101</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1.8</v>
+        <v>2.25</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.078</v>
@@ -4446,9 +4446,9 @@
         <v>0.012</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.281</v>
@@ -4838,9 +4838,9 @@
         <v>0.039</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>2.2</v>
+        <v>2.75</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1.371</v>
@@ -5230,9 +5230,9 @@
         <v>0.199</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2.344</v>
@@ -5622,9 +5622,9 @@
         <v>0.778</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>2.6</v>
+        <v>3.25</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3.609</v>
@@ -6014,9 +6014,9 @@
         <v>0.969</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4.514</v>
@@ -6406,9 +6406,9 @@
         <v>1.491</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>5.516</v>
@@ -6798,9 +6798,9 @@
         <v>1.994</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>6.398</v>
@@ -7190,9 +7190,9 @@
         <v>2.396</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>3.4</v>
+        <v>4.25</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>7.588</v>
@@ -7582,9 +7582,9 @@
         <v>2.908</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>8.205</v>
@@ -7974,9 +7974,9 @@
         <v>3.297</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>3.8</v>
+        <v>4.75</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>9.596</v>
@@ -8366,9 +8366,9 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>10.686</v>
@@ -8758,9 +8758,9 @@
         <v>4.075</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>4.2</v>
+        <v>5.25</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>11.544</v>
@@ -9150,9 +9150,9 @@
         <v>4.951</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>4.4</v>
+        <v>5.5</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>12.328</v>
@@ -9542,9 +9542,9 @@
         <v>5.556</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>4.6</v>
+        <v>5.75</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>13.551</v>
@@ -9934,9 +9934,9 @@
         <v>5.929</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>14.36</v>
@@ -10326,9 +10326,9 @@
         <v>6.494</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>5</v>
+        <v>6.25</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>12.23</v>
@@ -10718,9 +10718,9 @@
         <v>5.341</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>5.2</v>
+        <v>6.5</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>13.132</v>
@@ -11110,9 +11110,9 @@
         <v>5.867</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>5.4</v>
+        <v>6.75</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>14.392</v>
@@ -11502,9 +11502,9 @@
         <v>5.909</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>5.6</v>
+        <v>7</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>14.767</v>
@@ -11894,9 +11894,9 @@
         <v>6.333</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>5.8</v>
+        <v>7.25</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>14.824</v>
@@ -12286,9 +12286,9 @@
         <v>6.729</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>15.032</v>
@@ -12678,9 +12678,9 @@
         <v>6.809</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>6.2</v>
+        <v>7.75</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>15.168</v>
@@ -13070,9 +13070,9 @@
         <v>6.997</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>6.4</v>
+        <v>8</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>15.43</v>
@@ -13462,9 +13462,9 @@
         <v>6.693</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>6.6</v>
+        <v>8.25</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>15.741</v>
@@ -13854,9 +13854,9 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>6.8</v>
+        <v>8.5</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>15.819</v>
@@ -14246,9 +14246,9 @@
         <v>7.097</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>7</v>
+        <v>8.75</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>15.565</v>
@@ -14638,9 +14638,9 @@
         <v>6.939</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>7.2</v>
+        <v>9</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>15.738</v>
@@ -15030,9 +15030,9 @@
         <v>7.128</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>7.4</v>
+        <v>9.25</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>16.01</v>
@@ -15422,9 +15422,9 @@
         <v>7.052</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>7.6</v>
+        <v>9.5</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>15.783</v>
@@ -15814,9 +15814,9 @@
         <v>6.996</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>7.8</v>
+        <v>9.75</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>15.904</v>
@@ -16206,9 +16206,9 @@
         <v>7.132</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>16.185</v>
@@ -16598,9 +16598,9 @@
         <v>7.097</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>8.2</v>
+        <v>10.25</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>16.22</v>
@@ -16990,9 +16990,9 @@
         <v>7.148</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>8.4</v>
+        <v>10.5</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>15.889</v>
@@ -17382,9 +17382,9 @@
         <v>7.174</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>8.6</v>
+        <v>10.75</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>16.058</v>
@@ -17774,9 +17774,9 @@
         <v>7.042</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>8.8</v>
+        <v>11</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>15.845</v>
@@ -18166,9 +18166,9 @@
         <v>6.866</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>9</v>
+        <v>11.25</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>15.91</v>
@@ -18558,9 +18558,9 @@
         <v>7.022</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>9.2</v>
+        <v>11.5</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>16.088</v>
@@ -18950,9 +18950,9 @@
         <v>6.982</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>9.4</v>
+        <v>11.75</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>15.801</v>
@@ -19342,9 +19342,9 @@
         <v>7.222</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>9.6</v>
+        <v>12</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>16.274</v>
@@ -19734,9 +19734,9 @@
         <v>7.099</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>9.8</v>
+        <v>12.25</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>16.072</v>
@@ -20126,9 +20126,9 @@
         <v>6.93</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>16.118</v>
@@ -20518,9 +20518,9 @@
         <v>7.043</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>10.2</v>
+        <v>12.75</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>16.021</v>
@@ -20910,9 +20910,9 @@
         <v>6.894</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>10.4</v>
+        <v>13</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>15.947</v>
@@ -21302,9 +21302,9 @@
         <v>7.082</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>10.6</v>
+        <v>13.25</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>16.081</v>
@@ -21694,9 +21694,9 @@
         <v>6.772</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>10.8</v>
+        <v>13.5</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>16.104</v>
@@ -22086,9 +22086,9 @@
         <v>7.143</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>11</v>
+        <v>13.75</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>16.334</v>
@@ -22478,9 +22478,9 @@
         <v>6.956</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>11.2</v>
+        <v>14</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>15.902</v>
@@ -22870,9 +22870,9 @@
         <v>6.746</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>11.4</v>
+        <v>14.25</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>15.794</v>
@@ -23262,9 +23262,9 @@
         <v>6.773</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>11.6</v>
+        <v>14.5</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>15.426</v>
@@ -23654,9 +23654,9 @@
         <v>6.86</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>11.8</v>
+        <v>14.75</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>15.347</v>
@@ -24046,9 +24046,9 @@
         <v>6.775</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>15.4</v>
@@ -24438,9 +24438,9 @@
         <v>6.685</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>12.2</v>
+        <v>15.25</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>15.312</v>
@@ -24830,9 +24830,9 @@
         <v>6.995</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>12.4</v>
+        <v>15.5</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>15.144</v>
@@ -25222,9 +25222,9 @@
         <v>6.876</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>12.6</v>
+        <v>15.75</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>15.086</v>
@@ -25614,9 +25614,9 @@
         <v>6.996</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>12.8</v>
+        <v>16</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>15.397</v>
@@ -26006,9 +26006,9 @@
         <v>7.19</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>13</v>
+        <v>16.25</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>16.156</v>
@@ -26398,9 +26398,9 @@
         <v>7.266</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>13.2</v>
+        <v>16.5</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>16.414</v>
@@ -26790,9 +26790,9 @@
         <v>7.033</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>13.4</v>
+        <v>16.75</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>16.089</v>
@@ -27182,9 +27182,9 @@
         <v>7.167</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>13.6</v>
+        <v>17</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>15.686</v>
@@ -27574,9 +27574,9 @@
         <v>7.206</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>13.8</v>
+        <v>17.25</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>15.32</v>
@@ -27966,9 +27966,9 @@
         <v>7.097</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>14</v>
+        <v>17.5</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>15.401</v>
@@ -28358,9 +28358,9 @@
         <v>7.038</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>14.2</v>
+        <v>17.75</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>15.703</v>
@@ -28750,9 +28750,9 @@
         <v>7.223</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>14.4</v>
+        <v>18</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>15.884</v>
@@ -29142,9 +29142,9 @@
         <v>7.158</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>14.6</v>
+        <v>18.25</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>15.283</v>
@@ -29534,9 +29534,9 @@
         <v>7.097</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>14.8</v>
+        <v>18.5</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>15.411</v>
@@ -29926,9 +29926,9 @@
         <v>7.013</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>15</v>
+        <v>18.75</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>15.493</v>
@@ -30318,9 +30318,9 @@
         <v>7.048</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>15.2</v>
+        <v>19</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>15.46</v>
@@ -30710,9 +30710,9 @@
         <v>7.215</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>15.4</v>
+        <v>19.25</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>15.797</v>
@@ -31102,9 +31102,9 @@
         <v>7.079</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>15.6</v>
+        <v>19.5</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>15.322</v>
@@ -31494,9 +31494,9 @@
         <v>7.093</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>15.8</v>
+        <v>19.75</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>15.404</v>
@@ -31886,9 +31886,9 @@
         <v>7.093</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>15.115</v>
@@ -32278,9 +32278,9 @@
         <v>6.933</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>16.2</v>
+        <v>20.25</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>15.226</v>
@@ -32670,9 +32670,9 @@
         <v>7.031</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>16.4</v>
+        <v>20.5</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>15.181</v>
@@ -33062,9 +33062,9 @@
         <v>6.637</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>16.6</v>
+        <v>20.75</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>15.416</v>
@@ -33454,9 +33454,9 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>16.8</v>
+        <v>21</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>15.048</v>
@@ -33846,9 +33846,9 @@
         <v>6.872</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>17</v>
+        <v>21.25</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>15.122</v>
@@ -34238,9 +34238,9 @@
         <v>6.977</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>17.2</v>
+        <v>21.5</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>15.113</v>
@@ -34630,9 +34630,9 @@
         <v>6.874</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>17.4</v>
+        <v>21.75</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>15.08</v>
@@ -35022,9 +35022,9 @@
         <v>6.871</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>17.6</v>
+        <v>22</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>15.204</v>
@@ -35414,9 +35414,9 @@
         <v>6.848</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>17.8</v>
+        <v>22.25</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>15.486</v>
@@ -35806,9 +35806,9 @@
         <v>6.705</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>18</v>
+        <v>22.5</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>15.205</v>
@@ -36198,9 +36198,9 @@
         <v>6.953</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>18.2</v>
+        <v>22.75</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>15.318</v>
@@ -36590,9 +36590,9 @@
         <v>7.103</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>18.4</v>
+        <v>23</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>15.324</v>
@@ -36982,9 +36982,9 @@
         <v>7.052</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>18.6</v>
+        <v>23.25</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>15.439</v>
@@ -37374,9 +37374,9 @@
         <v>7.025</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>18.8</v>
+        <v>23.5</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>14.98</v>
@@ -37766,9 +37766,9 @@
         <v>6.938</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>19</v>
+        <v>23.75</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>15.376</v>
@@ -38158,9 +38158,9 @@
         <v>6.887</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>19.2</v>
+        <v>24</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>15.252</v>
@@ -38550,9 +38550,9 @@
         <v>7.096</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>19.4</v>
+        <v>24.25</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>15.153</v>
@@ -38942,9 +38942,9 @@
         <v>7.039</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>19.6</v>
+        <v>24.5</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>15.165</v>
@@ -39334,9 +39334,9 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
-        <v>19.8</v>
+        <v>24.75</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>15.17</v>
@@ -39726,9 +39726,9 @@
         <v>7.116</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>15.223</v>
@@ -40118,9 +40118,9 @@
         <v>7.043</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
-        <v>20.2</v>
+        <v>25.25</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>15.467</v>
@@ -40510,9 +40510,9 @@
         <v>7.12</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
-        <v>20.4</v>
+        <v>25.5</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>15.457</v>
@@ -40902,9 +40902,9 @@
         <v>6.968</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
-        <v>20.6</v>
+        <v>25.75</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>15.406</v>
@@ -41294,9 +41294,9 @@
         <v>6.898</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
-        <v>20.8</v>
+        <v>26</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>15.227</v>
@@ -41686,9 +41686,9 @@
         <v>6.896</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
-        <v>21</v>
+        <v>26.25</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>15.343</v>
@@ -42078,9 +42078,9 @@
         <v>6.904</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
-        <v>21.2</v>
+        <v>26.5</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>15.408</v>
@@ -42470,9 +42470,9 @@
         <v>6.784</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
-        <v>21.4</v>
+        <v>26.75</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>15.686</v>
@@ -42862,9 +42862,9 @@
         <v>7.125</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>15.224</v>
@@ -43254,9 +43254,9 @@
         <v>6.853</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
-        <v>21.8</v>
+        <v>27.25</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>15.108</v>
@@ -43646,9 +43646,9 @@
         <v>7.151</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
-        <v>22</v>
+        <v>27.5</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>15.407</v>
@@ -44038,9 +44038,9 @@
         <v>6.884</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
-        <v>22.2</v>
+        <v>27.75</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>15.39</v>
@@ -44430,9 +44430,9 @@
         <v>7.069</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
-        <v>22.4</v>
+        <v>28</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>15.425</v>
@@ -44822,9 +44822,9 @@
         <v>7.031</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
-        <v>22.6</v>
+        <v>28.25</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>15.387</v>
@@ -45214,9 +45214,9 @@
         <v>7.173</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
-        <v>22.8</v>
+        <v>28.5</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>15.268</v>
@@ -45606,9 +45606,9 @@
         <v>7.052</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
-        <v>23</v>
+        <v>28.75</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>15.327</v>
@@ -45998,9 +45998,9 @@
         <v>6.802</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
-        <v>23.2</v>
+        <v>29</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>15.401</v>
@@ -46390,9 +46390,9 @@
         <v>6.981</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
-        <v>23.4</v>
+        <v>29.25</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>15.333</v>
@@ -46782,9 +46782,9 @@
         <v>7.055</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
-        <v>23.6</v>
+        <v>29.5</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>15.277</v>
@@ -47174,9 +47174,9 @@
         <v>6.87</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
-        <v>23.8</v>
+        <v>29.75</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>15.293</v>

</xml_diff>